<commit_message>
feat: add GPA record access
</commit_message>
<xml_diff>
--- a/checklist_forStudent4.1.xlsx
+++ b/checklist_forStudent4.1.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
   <si>
     <t>Checklist of Group ____</t>
   </si>
@@ -1604,11 +1604,11 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.12727272727273" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1892,8 +1892,8 @@
       <c r="C21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="9">
-        <v>2</v>
+      <c r="D21" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="E21" s="9"/>
     </row>
@@ -1905,8 +1905,8 @@
       <c r="C22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="9">
-        <v>2</v>
+      <c r="D22" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="E22" s="9"/>
     </row>
@@ -2011,8 +2011,8 @@
       <c r="C30" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="9">
-        <v>2</v>
+      <c r="D30" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="E30" s="9"/>
     </row>

</xml_diff>

<commit_message>
now e-admin can load and show one policy
</commit_message>
<xml_diff>
--- a/checklist_forStudent4.1.xlsx
+++ b/checklist_forStudent4.1.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18825\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDW\project_v1_36094\EDBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF23281-8E78-4FA6-9720-F9C7D9EC47B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E511E0-017A-458B-8D5E-3B5A276853CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GoTb5jAQ2RfFIzX11kNVEF8Fd934VL15DZlgrmJmecMgr9kSgVUfyyT/VVsHiN395k+zFb2SSoLq5VpW+lu+ew==" workbookSaltValue="DxxokmHZpEtf+xpnLfpRyQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
   <si>
     <t>Checklist of Group ____</t>
   </si>
@@ -504,16 +504,20 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -522,10 +526,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1014,28 +1014,28 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="105.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" customWidth="1"/>
-    <col min="5" max="5" width="27.90625" customWidth="1"/>
+    <col min="1" max="1" width="18.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.75" style="2" customWidth="1"/>
+    <col min="3" max="3" width="105.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
+    <col min="5" max="5" width="27.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" ht="20.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -1077,7 +1077,7 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1086,13 +1086,13 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="13" t="s">
         <v>63</v>
       </c>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="17"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1105,7 +1105,7 @@
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="17"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1118,7 +1118,7 @@
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="17"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
@@ -1131,19 +1131,19 @@
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="11">
-        <v>1</v>
+      <c r="D9" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="28">
+    <row r="10" spans="1:5" ht="27">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="34" customHeight="1">
+    <row r="11" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" ht="53.15" customHeight="1">
+    <row r="12" spans="1:5" ht="53.1" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="4" t="s">
         <v>7</v>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="52" customHeight="1">
+    <row r="13" spans="1:5" ht="51.95" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="4" t="s">
         <v>12</v>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" ht="28">
+    <row r="23" spans="1:5" ht="27">
       <c r="A23" s="14"/>
       <c r="B23" s="4" t="s">
         <v>26</v>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" ht="20.149999999999999" customHeight="1">
+    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="15"/>
       <c r="B32" s="4" t="s">
         <v>31</v>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" ht="20.149999999999999" customHeight="1">
+    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="15"/>
       <c r="B33" s="4" t="s">
         <v>51</v>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:5" ht="37" customHeight="1">
+    <row r="35" spans="1:5" ht="36.950000000000003" customHeight="1">
       <c r="A35" s="15"/>
       <c r="B35" s="4" t="s">
         <v>55</v>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" ht="35.15" customHeight="1">
+    <row r="37" spans="1:5" ht="35.1" customHeight="1">
       <c r="A37" s="15"/>
       <c r="B37" s="4" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
add update to teacher.py
</commit_message>
<xml_diff>
--- a/checklist_forStudent4.1.xlsx
+++ b/checklist_forStudent4.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDW\project_v1_36094\EDBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E511E0-017A-458B-8D5E-3B5A276853CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93DD332-60DA-4324-A7A6-8A4BB0DF2FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GoTb5jAQ2RfFIzX11kNVEF8Fd934VL15DZlgrmJmecMgr9kSgVUfyyT/VVsHiN395k+zFb2SSoLq5VpW+lu+ew==" workbookSaltValue="DxxokmHZpEtf+xpnLfpRyQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>Checklist of Group ____</t>
   </si>
@@ -1014,7 +1014,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
@@ -1220,8 +1220,8 @@
       <c r="C15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="8">
-        <v>1</v>
+      <c r="D15" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="E15" s="8"/>
     </row>

</xml_diff>

<commit_message>
add download and show logic to oconvener.py
</commit_message>
<xml_diff>
--- a/checklist_forStudent4.1.xlsx
+++ b/checklist_forStudent4.1.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDW\project_v1_36094\EDBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93DD332-60DA-4324-A7A6-8A4BB0DF2FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD4D355-A440-4DCE-B096-8CFB6006433D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GoTb5jAQ2RfFIzX11kNVEF8Fd934VL15DZlgrmJmecMgr9kSgVUfyyT/VVsHiN395k+zFb2SSoLq5VpW+lu+ew==" workbookSaltValue="DxxokmHZpEtf+xpnLfpRyQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="4005" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
   <si>
     <t>Checklist of Group ____</t>
   </si>
@@ -1011,10 +1011,10 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
@@ -1458,8 +1458,8 @@
       <c r="C33" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="8">
-        <v>1</v>
+      <c r="D33" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="E33" s="8"/>
     </row>

</xml_diff>

<commit_message>
add view logic for student and teacher dashboard
</commit_message>
<xml_diff>
--- a/checklist_forStudent4.1.xlsx
+++ b/checklist_forStudent4.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDW\project_v1_36094\EDBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD4D355-A440-4DCE-B096-8CFB6006433D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB57DE44-2FB9-4FAA-87B7-B9603FA950CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GoTb5jAQ2RfFIzX11kNVEF8Fd934VL15DZlgrmJmecMgr9kSgVUfyyT/VVsHiN395k+zFb2SSoLq5VpW+lu+ew==" workbookSaltValue="DxxokmHZpEtf+xpnLfpRyQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="5835" yWindow="4005" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
   <si>
     <t>Checklist of Group ____</t>
   </si>
@@ -1011,10 +1011,10 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
@@ -1432,8 +1432,8 @@
       <c r="C31" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="8">
-        <v>1</v>
+      <c r="D31" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="E31" s="8"/>
     </row>

</xml_diff>

<commit_message>
setEadmin and seek help
</commit_message>
<xml_diff>
--- a/checklist_forStudent4.1.xlsx
+++ b/checklist_forStudent4.1.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDW\project_v1_36094\EDBA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EDBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB57DE44-2FB9-4FAA-87B7-B9603FA950CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39251320-703E-4F85-8FB7-C30B5471EA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GoTb5jAQ2RfFIzX11kNVEF8Fd934VL15DZlgrmJmecMgr9kSgVUfyyT/VVsHiN395k+zFb2SSoLq5VpW+lu+ew==" workbookSaltValue="DxxokmHZpEtf+xpnLfpRyQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="4005" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3744" yWindow="4368" windowWidth="19176" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
   <si>
     <t>Checklist of Group ____</t>
   </si>
@@ -313,6 +313,10 @@
   </si>
   <si>
     <t>1 done</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>3done</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -1011,22 +1015,22 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="18.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.75" style="2" customWidth="1"/>
-    <col min="3" max="3" width="105.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.375" customWidth="1"/>
-    <col min="5" max="5" width="27.875" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="105.36328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" customWidth="1"/>
+    <col min="5" max="5" width="27.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25">
+    <row r="1" spans="1:5" ht="21">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +1039,7 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -1058,12 +1062,12 @@
       <c r="C3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="8">
-        <v>3</v>
+      <c r="D3" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -1143,7 +1147,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="27">
+    <row r="10" spans="1:5" ht="28">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1158,7 +1162,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="33.950000000000003" customHeight="1">
+    <row r="11" spans="1:5" ht="34" customHeight="1">
       <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
@@ -1173,7 +1177,7 @@
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" ht="53.1" customHeight="1">
+    <row r="12" spans="1:5" ht="53.15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="4" t="s">
         <v>7</v>
@@ -1186,7 +1190,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="51.95" customHeight="1">
+    <row r="13" spans="1:5" ht="52" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="4" t="s">
         <v>12</v>
@@ -1318,7 +1322,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" ht="27">
+    <row r="23" spans="1:5" ht="28">
       <c r="A23" s="14"/>
       <c r="B23" s="4" t="s">
         <v>26</v>
@@ -1393,8 +1397,8 @@
       <c r="C28" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="8">
-        <v>3</v>
+      <c r="D28" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="E28" s="8"/>
     </row>
@@ -1437,7 +1441,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="32" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A32" s="15"/>
       <c r="B32" s="4" t="s">
         <v>31</v>
@@ -1450,7 +1454,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="33" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A33" s="15"/>
       <c r="B33" s="4" t="s">
         <v>51</v>
@@ -1476,7 +1480,7 @@
       </c>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:5" ht="36.950000000000003" customHeight="1">
+    <row r="35" spans="1:5" ht="37" customHeight="1">
       <c r="A35" s="15"/>
       <c r="B35" s="4" t="s">
         <v>55</v>
@@ -1502,7 +1506,7 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" ht="35.1" customHeight="1">
+    <row r="37" spans="1:5" ht="35.15" customHeight="1">
       <c r="A37" s="15"/>
       <c r="B37" s="4" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
helprequest star need to be done
</commit_message>
<xml_diff>
--- a/checklist_forStudent4.1.xlsx
+++ b/checklist_forStudent4.1.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EDBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39251320-703E-4F85-8FB7-C30B5471EA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B42D7B-954E-42C3-90DC-078FFB4C06C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GoTb5jAQ2RfFIzX11kNVEF8Fd934VL15DZlgrmJmecMgr9kSgVUfyyT/VVsHiN395k+zFb2SSoLq5VpW+lu+ew==" workbookSaltValue="DxxokmHZpEtf+xpnLfpRyQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="3744" yWindow="4368" windowWidth="19176" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="65">
   <si>
     <t>Checklist of Group ____</t>
   </si>
@@ -1015,22 +1015,22 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="105.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" customWidth="1"/>
-    <col min="5" max="5" width="27.90625" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="105.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
+    <row r="1" spans="1:5" ht="20.399999999999999">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -1075,8 +1075,8 @@
       <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8">
-        <v>3</v>
+      <c r="D4" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="E4" s="8"/>
     </row>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="28">
+    <row r="10" spans="1:5" ht="28.8">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1162,7 +1162,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="34" customHeight="1">
+    <row r="11" spans="1:5" ht="34.049999999999997" customHeight="1">
       <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" ht="53.15" customHeight="1">
+    <row r="12" spans="1:5" ht="53.1" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="4" t="s">
         <v>7</v>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="52" customHeight="1">
+    <row r="13" spans="1:5" ht="52.05" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="4" t="s">
         <v>12</v>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" ht="28">
+    <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="14"/>
       <c r="B23" s="4" t="s">
         <v>26</v>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" ht="20.149999999999999" customHeight="1">
+    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="15"/>
       <c r="B32" s="4" t="s">
         <v>31</v>
@@ -1454,7 +1454,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" ht="20.149999999999999" customHeight="1">
+    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="15"/>
       <c r="B33" s="4" t="s">
         <v>51</v>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:5" ht="37" customHeight="1">
+    <row r="35" spans="1:5" ht="37.049999999999997" customHeight="1">
       <c r="A35" s="15"/>
       <c r="B35" s="4" t="s">
         <v>55</v>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" ht="35.15" customHeight="1">
+    <row r="37" spans="1:5" ht="35.1" customHeight="1">
       <c r="A37" s="15"/>
       <c r="B37" s="4" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
add view thesis logic to teacher
</commit_message>
<xml_diff>
--- a/checklist_forStudent4.1.xlsx
+++ b/checklist_forStudent4.1.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EDBA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDW\project_v1_36094\EDBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39251320-703E-4F85-8FB7-C30B5471EA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADD787D-977D-4428-B411-E6F71DC10228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GoTb5jAQ2RfFIzX11kNVEF8Fd934VL15DZlgrmJmecMgr9kSgVUfyyT/VVsHiN395k+zFb2SSoLq5VpW+lu+ew==" workbookSaltValue="DxxokmHZpEtf+xpnLfpRyQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="3744" yWindow="4368" windowWidth="19176" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="4005" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1015,22 +1015,22 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="105.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" customWidth="1"/>
-    <col min="5" max="5" width="27.90625" customWidth="1"/>
+    <col min="1" max="1" width="18.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.75" style="2" customWidth="1"/>
+    <col min="3" max="3" width="105.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
+    <col min="5" max="5" width="27.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
+    <row r="1" spans="1:5" ht="20.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1039,7 +1039,7 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="28">
+    <row r="10" spans="1:5" ht="27">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1162,7 +1162,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="34" customHeight="1">
+    <row r="11" spans="1:5" ht="33.950000000000003" customHeight="1">
       <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" ht="53.15" customHeight="1">
+    <row r="12" spans="1:5" ht="53.1" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="4" t="s">
         <v>7</v>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="52" customHeight="1">
+    <row r="13" spans="1:5" ht="51.95" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="4" t="s">
         <v>12</v>
@@ -1251,7 +1251,7 @@
         <v>30</v>
       </c>
       <c r="D17" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17" s="8"/>
     </row>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" ht="28">
+    <row r="23" spans="1:5" ht="27">
       <c r="A23" s="14"/>
       <c r="B23" s="4" t="s">
         <v>26</v>
@@ -1331,7 +1331,7 @@
         <v>38</v>
       </c>
       <c r="D23" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E23" s="8"/>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" ht="20.149999999999999" customHeight="1">
+    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="15"/>
       <c r="B32" s="4" t="s">
         <v>31</v>
@@ -1454,7 +1454,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" ht="20.149999999999999" customHeight="1">
+    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="15"/>
       <c r="B33" s="4" t="s">
         <v>51</v>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:5" ht="37" customHeight="1">
+    <row r="35" spans="1:5" ht="36.950000000000003" customHeight="1">
       <c r="A35" s="15"/>
       <c r="B35" s="4" t="s">
         <v>55</v>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" ht="35.15" customHeight="1">
+    <row r="37" spans="1:5" ht="35.1" customHeight="1">
       <c r="A37" s="15"/>
       <c r="B37" s="4" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
add bach process for oconvener
</commit_message>
<xml_diff>
--- a/checklist_forStudent4.1.xlsx
+++ b/checklist_forStudent4.1.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDW\project_v1_36094\EDBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C77B5DA-7BD3-4624-BBC8-479278BB52E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2D3E6A-4DB0-4B65-9FCE-CDA541084D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GoTb5jAQ2RfFIzX11kNVEF8Fd934VL15DZlgrmJmecMgr9kSgVUfyyT/VVsHiN395k+zFb2SSoLq5VpW+lu+ew==" workbookSaltValue="DxxokmHZpEtf+xpnLfpRyQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="4350" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8805" yWindow="3015" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
   <si>
     <t>Checklist of Group ____</t>
   </si>
@@ -1018,7 +1018,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
@@ -1198,8 +1198,8 @@
       <c r="C13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="8">
-        <v>1</v>
+      <c r="D13" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="E13" s="8"/>
     </row>

</xml_diff>

<commit_message>
now oconvener can decide what functions user can access
</commit_message>
<xml_diff>
--- a/checklist_forStudent4.1.xlsx
+++ b/checklist_forStudent4.1.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EDBA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDW\project_v1_36094\EDBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA65CD7-4860-4519-9022-1989136C4E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0949E2E2-9846-4BC5-99E2-04931427A0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GoTb5jAQ2RfFIzX11kNVEF8Fd934VL15DZlgrmJmecMgr9kSgVUfyyT/VVsHiN395k+zFb2SSoLq5VpW+lu+ew==" workbookSaltValue="DxxokmHZpEtf+xpnLfpRyQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="30984" windowHeight="16824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
   <si>
     <t>Checklist of Group ____</t>
   </si>
@@ -520,6 +520,10 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -538,10 +542,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1026,37 +1026,37 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="105.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" customWidth="1"/>
-    <col min="5" max="5" width="27.90625" customWidth="1"/>
+    <col min="1" max="1" width="18.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.75" style="2" customWidth="1"/>
+    <col min="3" max="3" width="105.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
+    <col min="5" max="5" width="27.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:5" ht="20.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="13" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" ht="15">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1065,7 +1065,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1079,8 +1079,8 @@
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" ht="17.149999999999999" customHeight="1">
-      <c r="A4" s="14"/>
+    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1093,7 +1093,7 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1108,7 +1108,7 @@
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="17"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1121,7 +1121,7 @@
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="17"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1134,7 +1134,7 @@
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="17"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
@@ -1147,19 +1147,19 @@
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="13" t="s">
         <v>66</v>
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="28">
+    <row r="10" spans="1:5" ht="27">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1175,7 +1175,7 @@
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="34.15" customHeight="1">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1184,13 +1184,13 @@
       <c r="C11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="8">
-        <v>1</v>
+      <c r="D11" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" ht="53.15" customHeight="1">
-      <c r="A12" s="14"/>
+    <row r="12" spans="1:5" ht="53.1" customHeight="1">
+      <c r="A12" s="15"/>
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1203,7 +1203,7 @@
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" ht="52.15" customHeight="1">
-      <c r="A13" s="14"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
@@ -1216,7 +1216,7 @@
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1">
-      <c r="A14" s="14"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1229,7 +1229,7 @@
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1">
-      <c r="A15" s="14"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
@@ -1242,7 +1242,7 @@
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1">
-      <c r="A16" s="14"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
@@ -1255,7 +1255,7 @@
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" ht="72" customHeight="1">
-      <c r="A17" s="14"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
@@ -1268,7 +1268,7 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="4" t="s">
         <v>31</v>
       </c>
@@ -1281,7 +1281,7 @@
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1296,7 +1296,7 @@
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="13"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1309,7 +1309,7 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="13"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="4" t="s">
         <v>12</v>
       </c>
@@ -1322,7 +1322,7 @@
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1">
-      <c r="A22" s="13"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="4" t="s">
         <v>15</v>
       </c>
@@ -1334,8 +1334,8 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" ht="28">
-      <c r="A23" s="13"/>
+    <row r="23" spans="1:5" ht="27">
+      <c r="A23" s="14"/>
       <c r="B23" s="4" t="s">
         <v>26</v>
       </c>
@@ -1348,7 +1348,7 @@
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="13"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="4" t="s">
         <v>28</v>
       </c>
@@ -1361,7 +1361,7 @@
       <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="13"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="4" t="s">
         <v>40</v>
       </c>
@@ -1374,7 +1374,7 @@
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1">
-      <c r="A26" s="13"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="4" t="s">
         <v>42</v>
       </c>
@@ -1387,7 +1387,7 @@
       <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="15" t="s">
         <v>44</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -1402,7 +1402,7 @@
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="14"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="4" t="s">
         <v>7</v>
       </c>
@@ -1415,7 +1415,7 @@
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" ht="36" customHeight="1">
-      <c r="A29" s="14"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="4" t="s">
         <v>12</v>
       </c>
@@ -1428,7 +1428,7 @@
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="14"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="4" t="s">
         <v>15</v>
       </c>
@@ -1441,7 +1441,7 @@
       <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="14"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="4" t="s">
         <v>17</v>
       </c>
@@ -1453,8 +1453,8 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" ht="20.149999999999999" customHeight="1">
-      <c r="A32" s="14"/>
+    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="15"/>
       <c r="B32" s="4" t="s">
         <v>31</v>
       </c>
@@ -1466,8 +1466,8 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" ht="20.149999999999999" customHeight="1">
-      <c r="A33" s="14"/>
+    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A33" s="15"/>
       <c r="B33" s="4" t="s">
         <v>51</v>
       </c>
@@ -1480,7 +1480,7 @@
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="14"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="4" t="s">
         <v>53</v>
       </c>
@@ -1493,7 +1493,7 @@
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5" ht="37.15" customHeight="1">
-      <c r="A35" s="14"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="4" t="s">
         <v>55</v>
       </c>
@@ -1506,7 +1506,7 @@
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="14"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="4" t="s">
         <v>57</v>
       </c>
@@ -1518,8 +1518,8 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" ht="35.15" customHeight="1">
-      <c r="A37" s="14"/>
+    <row r="37" spans="1:5" ht="35.1" customHeight="1">
+      <c r="A37" s="15"/>
       <c r="B37" s="4" t="s">
         <v>59</v>
       </c>
@@ -1532,7 +1532,7 @@
       <c r="E37" s="8"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="14"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="4" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
add charge logic to service
</commit_message>
<xml_diff>
--- a/checklist_forStudent4.1.xlsx
+++ b/checklist_forStudent4.1.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDW\project_v1_36094\EDBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8829B739-7D12-48A7-AFA5-BDE6C61AC3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51859D9B-058C-401D-8254-3FF8665B7A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GoTb5jAQ2RfFIzX11kNVEF8Fd934VL15DZlgrmJmecMgr9kSgVUfyyT/VVsHiN395k+zFb2SSoLq5VpW+lu+ew==" workbookSaltValue="DxxokmHZpEtf+xpnLfpRyQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="5070" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
   <si>
     <t>Checklist of Group ____</t>
   </si>
@@ -1027,10 +1027,10 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
@@ -1142,7 +1142,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" s="8"/>
     </row>
@@ -1250,7 +1250,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16" s="8"/>
     </row>
@@ -1500,8 +1500,8 @@
       <c r="C35" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="8">
-        <v>3</v>
+      <c r="D35" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="E35" s="8"/>
     </row>
@@ -1513,8 +1513,8 @@
       <c r="C36" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="8">
-        <v>3</v>
+      <c r="D36" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="E36" s="8"/>
     </row>
@@ -1526,8 +1526,8 @@
       <c r="C37" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="8">
-        <v>3</v>
+      <c r="D37" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="E37" s="8"/>
     </row>
@@ -1539,8 +1539,8 @@
       <c r="C38" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="11">
-        <v>3</v>
+      <c r="D38" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="E38" s="8"/>
     </row>

</xml_diff>

<commit_message>
pay after and before
</commit_message>
<xml_diff>
--- a/checklist_forStudent4.1.xlsx
+++ b/checklist_forStudent4.1.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SDW\project_v1_36094\EDBA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EDBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51859D9B-058C-401D-8254-3FF8665B7A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F23B9DD-11DB-4EB1-8E2D-1F1B3231F1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GoTb5jAQ2RfFIzX11kNVEF8Fd934VL15DZlgrmJmecMgr9kSgVUfyyT/VVsHiN395k+zFb2SSoLq5VpW+lu+ew==" workbookSaltValue="DxxokmHZpEtf+xpnLfpRyQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="5070" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
   <si>
     <t>Checklist of Group ____</t>
   </si>
@@ -1027,22 +1027,22 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="18.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.75" style="2" customWidth="1"/>
-    <col min="3" max="3" width="105.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.375" customWidth="1"/>
-    <col min="5" max="5" width="27.875" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="105.36328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" customWidth="1"/>
+    <col min="5" max="5" width="27.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25">
+    <row r="1" spans="1:5" ht="21">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1051,7 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -1141,8 +1141,8 @@
       <c r="C8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="8">
-        <v>3</v>
+      <c r="D8" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="E8" s="8"/>
     </row>
@@ -1159,7 +1159,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="27">
+    <row r="10" spans="1:5" ht="28">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="34.15" customHeight="1">
+    <row r="11" spans="1:5" ht="34.25" customHeight="1">
       <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" ht="53.1" customHeight="1">
+    <row r="12" spans="1:5" ht="53.15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="4" t="s">
         <v>7</v>
@@ -1202,7 +1202,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="52.15" customHeight="1">
+    <row r="13" spans="1:5" ht="52.25" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="4" t="s">
         <v>12</v>
@@ -1249,8 +1249,8 @@
       <c r="C16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="8">
-        <v>3</v>
+      <c r="D16" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="E16" s="8"/>
     </row>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" ht="27">
+    <row r="23" spans="1:5" ht="28">
       <c r="A23" s="14"/>
       <c r="B23" s="4" t="s">
         <v>26</v>
@@ -1355,8 +1355,8 @@
       <c r="C24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="8">
-        <v>3</v>
+      <c r="D24" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="E24" s="8"/>
     </row>
@@ -1381,8 +1381,8 @@
       <c r="C26" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="8">
-        <v>3</v>
+      <c r="D26" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="E26" s="8"/>
     </row>
@@ -1422,8 +1422,8 @@
       <c r="C29" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="8">
-        <v>3</v>
+      <c r="D29" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="E29" s="8"/>
     </row>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="32" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A32" s="15"/>
       <c r="B32" s="4" t="s">
         <v>31</v>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="33" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A33" s="15"/>
       <c r="B33" s="4" t="s">
         <v>51</v>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:5" ht="37.15" customHeight="1">
+    <row r="35" spans="1:5" ht="37.25" customHeight="1">
       <c r="A35" s="15"/>
       <c r="B35" s="4" t="s">
         <v>55</v>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" ht="35.1" customHeight="1">
+    <row r="37" spans="1:5" ht="35.15" customHeight="1">
       <c r="A37" s="15"/>
       <c r="B37" s="4" t="s">
         <v>59</v>

</xml_diff>